<commit_message>
Add brands to description
</commit_message>
<xml_diff>
--- a/conformance_file_descriptions.xlsx
+++ b/conformance_file_descriptions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Test Content" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="137">
   <si>
     <t>File ID</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Input bitstreams</t>
   </si>
   <si>
+    <t>Brands</t>
+  </si>
+  <si>
     <t>C001</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
     <t>B001, B002</t>
   </si>
   <si>
+    <t>heic, hevc, mif1, msf1</t>
+  </si>
+  <si>
     <t>C002</t>
   </si>
   <si>
@@ -49,6 +55,9 @@
     <t>B001</t>
   </si>
   <si>
+    <t>heic, mif1</t>
+  </si>
+  <si>
     <t>C003</t>
   </si>
   <si>
@@ -217,6 +226,9 @@
     <t>B002</t>
   </si>
   <si>
+    <t>hevc, msf1</t>
+  </si>
+  <si>
     <t>C027</t>
   </si>
   <si>
@@ -277,6 +289,9 @@
     <t>B013</t>
   </si>
   <si>
+    <t>mif1</t>
+  </si>
+  <si>
     <t>C036</t>
   </si>
   <si>
@@ -317,9 +332,6 @@
   </si>
   <si>
     <t>B019</t>
-  </si>
-  <si>
-    <t>hevc, msf1</t>
   </si>
   <si>
     <t>Bitstream ID</t>
@@ -623,19 +635,20 @@
   </sheetPr>
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B67" activeCellId="0" sqref="B67"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="90.085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.2024291497976"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="90.9433198380567"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.6315789473684"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4008097165992"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -645,657 +658,789 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="D17" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="D23" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0"/>
     </row>
+    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0"/>
+    </row>
+    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0"/>
+    </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reduce sizes of some input HEVC bitstreams.
This is done to reduce generated conformance file sizes.

Truncate B002.265 bitstream from 80 to 8 frames.
Truncate B012.265 bitstream from 30 to 8 frames.
Truncate B010.265 bitstream from 80 to 16 frames.
Truncate B011.265 bitstream from 80 to 16 frames.
Modify edit lists C029, C036, C037 and C038 correspondingly.
</commit_message>
<xml_diff>
--- a/conformance_file_descriptions.xlsx
+++ b/conformance_file_descriptions.xlsx
@@ -22,415 +22,415 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="137">
   <si>
-    <t>File ID</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Input bitstreams</t>
-  </si>
-  <si>
-    <t>Brands</t>
-  </si>
-  <si>
-    <t>C001</t>
-  </si>
-  <si>
-    <t>A file with an image item and an image sequence, using file offset, first image item a s primary image</t>
-  </si>
-  <si>
-    <t>B001, B002</t>
-  </si>
-  <si>
-    <t>heic, hevc, mif1, msf1</t>
-  </si>
-  <si>
-    <t>C002</t>
-  </si>
-  <si>
-    <t>file with 1 image item</t>
-  </si>
-  <si>
-    <t>B001</t>
-  </si>
-  <si>
-    <t>heic, mif1</t>
-  </si>
-  <si>
-    <t>C003</t>
-  </si>
-  <si>
-    <t>file with 2 image items</t>
-  </si>
-  <si>
-    <t>B001, B003</t>
-  </si>
-  <si>
-    <t>C004</t>
-  </si>
-  <si>
-    <t>file with 10 image items</t>
-  </si>
-  <si>
-    <t>B004</t>
-  </si>
-  <si>
-    <t>C005</t>
-  </si>
-  <si>
-    <t>thumbnail image as primary : one image and a thumbnail image</t>
-  </si>
-  <si>
-    <t>B001, B005</t>
-  </si>
-  <si>
-    <t>C006</t>
-  </si>
-  <si>
-    <t>auxiliary image as a primary item</t>
-  </si>
-  <si>
-    <t>B001, B006</t>
-  </si>
-  <si>
-    <t>C007</t>
-  </si>
-  <si>
-    <t>contains a derived image of type "grid" from first 4 images and it is set as primary image item</t>
-  </si>
-  <si>
-    <t>C008</t>
-  </si>
-  <si>
-    <t>contains a derived image which is a rotated image of B003 input image and it is set as primary image item.</t>
-  </si>
-  <si>
-    <t>C009</t>
-  </si>
-  <si>
-    <t>One of the images is set as hidden image.</t>
-  </si>
-  <si>
-    <t>C010</t>
-  </si>
-  <si>
-    <t>Make these two items "altr" grouped.</t>
-  </si>
-  <si>
-    <t>C011</t>
-  </si>
-  <si>
-    <t>Make these items hidden and then "altr" grouped</t>
-  </si>
-  <si>
-    <t>C012</t>
-  </si>
-  <si>
-    <t>file with 10 images, 10 thumbnails and 1 additional image item. Additional image item is pre-derived from two thumbnail images.</t>
-  </si>
-  <si>
-    <t>B004, B007, B001</t>
-  </si>
-  <si>
-    <t>C013</t>
-  </si>
-  <si>
-    <t>clap box to crop (0,0,300,300) on 2 images  in C003</t>
-  </si>
-  <si>
-    <t>C014</t>
-  </si>
-  <si>
-    <t>irot box to rotate 90 degrees applied to one image  in C003 and then crop the image. Then, make that image a primary item. Add another irot box of 180 degree rotation and apply to B003 as another image item.</t>
-  </si>
-  <si>
-    <t>C015</t>
-  </si>
-  <si>
-    <t>Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (160,240). Canvas fill is 0 (transparent)</t>
-  </si>
-  <si>
-    <t>C016</t>
-  </si>
-  <si>
-    <t>Contains a derived image item where the 1st image item is overlaid on a canvas of black. Total output w,h = 1440, 960. image on top of the first one with an offset of (80,120).</t>
-  </si>
-  <si>
-    <t>C017</t>
-  </si>
-  <si>
-    <t>Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (640,360). Canvas fill is 65535</t>
-  </si>
-  <si>
-    <t>B008,B009</t>
-  </si>
-  <si>
-    <t>C018</t>
-  </si>
-  <si>
-    <t>Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (640,360). Canvas fill is 0</t>
-  </si>
-  <si>
-    <t>C019</t>
-  </si>
-  <si>
-    <t>Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (-320,-180). Canvas fill is 65535</t>
-  </si>
-  <si>
-    <t>C020</t>
-  </si>
-  <si>
-    <t>Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (-640,-360). Canvas fill is 65535</t>
-  </si>
-  <si>
-    <t>C021</t>
-  </si>
-  <si>
-    <t>Contains a derived image item where the  image item is overlaid on a canvas of dimensions w,h = 640, 360.Second image on top of the first one with an offset of (-640,-360). Canvas fill is 65535.</t>
-  </si>
-  <si>
-    <t>C022</t>
-  </si>
-  <si>
-    <t>contains a derived image of type "grid" from first 4 images and it is set as primary image item. Output width and height = (1449, 960)</t>
-  </si>
-  <si>
-    <t>C023</t>
-  </si>
-  <si>
-    <t>containes a grid of 4 derived images which are cropped to (640,360)</t>
-  </si>
-  <si>
-    <t>C024</t>
-  </si>
-  <si>
-    <t>contains a grid of 1x1 dimension</t>
-  </si>
-  <si>
-    <t>C025</t>
-  </si>
-  <si>
-    <t>contains a grid of 3x2 dimension. Uses the first 6 frames.</t>
-  </si>
-  <si>
-    <t>B007</t>
-  </si>
-  <si>
-    <t>C026</t>
-  </si>
-  <si>
-    <t>a file with an image sequence only</t>
-  </si>
-  <si>
-    <t>B002</t>
-  </si>
-  <si>
-    <t>hevc, msf1</t>
-  </si>
-  <si>
-    <t>C027</t>
-  </si>
-  <si>
-    <t>a file with image sequence track with inter prediction but no intra-pred in inter-predicted frames</t>
-  </si>
-  <si>
-    <t>B010</t>
-  </si>
-  <si>
-    <t>C028</t>
-  </si>
-  <si>
-    <t>a file with image sequence track with inter prediction with intra-pred in inter-predicted frames</t>
-  </si>
-  <si>
-    <t>B011</t>
-  </si>
-  <si>
-    <t>C029</t>
-  </si>
-  <si>
-    <t>A file with an edit list of playing the first 10 samples twice</t>
-  </si>
-  <si>
-    <t>C030</t>
-  </si>
-  <si>
-    <t>A file with an edit list of a pause at the beginning</t>
-  </si>
-  <si>
-    <t>C031</t>
-  </si>
-  <si>
-    <t>a file with image sequence track and a video track</t>
-  </si>
-  <si>
-    <t>C032</t>
-  </si>
-  <si>
-    <t>a file with a pict track and a thumbnail track also alternate groups indicated</t>
-  </si>
-  <si>
-    <t>B002, B012</t>
-  </si>
-  <si>
-    <t>C033</t>
-  </si>
-  <si>
-    <t>a file with a pict track and a thumbnail track with no alternate groups indicated</t>
-  </si>
-  <si>
-    <t>C034</t>
-  </si>
-  <si>
-    <t>A file with EXIF metadata present in it</t>
-  </si>
-  <si>
-    <t>B013</t>
-  </si>
-  <si>
-    <t>mif1</t>
-  </si>
-  <si>
-    <t>C036</t>
-  </si>
-  <si>
-    <t>A file with an all-intra encoded video track and an edit list with repeat flag, repeating an integer number of times.</t>
-  </si>
-  <si>
-    <t>C037</t>
-  </si>
-  <si>
-    <t>A file with an all-intra encoded video track and an edit list with repeat flag, repeating a non-integer number of times.</t>
-  </si>
-  <si>
-    <t>C038</t>
-  </si>
-  <si>
-    <t>A file with an all-intra encoded video track and an edit list with a repeat flag, repeating for infinite number of times</t>
-  </si>
-  <si>
-    <t>C039</t>
-  </si>
-  <si>
-    <t>Add another image item to C014 configuration with crop and rotate operation on top of already present crop-and-rotated image item and make that item a primary item.</t>
-  </si>
-  <si>
-    <t>C040</t>
-  </si>
-  <si>
-    <t>Pre-derived coded image. First 2x2 grid image as pre-derived coded image</t>
-  </si>
-  <si>
-    <t>B014, B015, B016, B017, B018</t>
-  </si>
-  <si>
-    <t>C041</t>
-  </si>
-  <si>
-    <t>A file with a non-display sample (the first Intra frame) and 8 more inter-frames in it</t>
-  </si>
-  <si>
-    <t>B019</t>
-  </si>
-  <si>
-    <t>Bitstream ID</t>
-  </si>
-  <si>
-    <t>Same input content as bitstream:</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile Intra encoded Frame (1280x720 resolution)</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile all-intra encoded bitstream made up of 80 frames (1280x720 resolution)</t>
-  </si>
-  <si>
-    <t>B003</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile all-intra encoded bitstream made up of 10 frames (1280x720 resolution)</t>
-  </si>
-  <si>
-    <t>B005</t>
-  </si>
-  <si>
-    <t>Thumbail image - HEVC Main Profile Intra encoded Frame (128x72 resolution)</t>
-  </si>
-  <si>
-    <t>B006</t>
-  </si>
-  <si>
-    <t>Alpha mask of the image - HEVC Main Profile Intra encoded Frame (1280x720 resolution)</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile all-intra encoded bitstream made up of 10 frames (128x72 resolution)</t>
-  </si>
-  <si>
-    <t>B008</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile all-Intra encoded Frame (640x360 resolution)</t>
-  </si>
-  <si>
-    <t>B009</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile Intra encoded Frame (640x360 resolution)</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile inter-prediction used bitstream (1280x720 resolution), but no intra-prediction in the inter-predicted frames.</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile inter-prediction used bitstream (1280x720 resolution), with intra-prediction used in the inter-predicted frames.</t>
-  </si>
-  <si>
-    <t>B012</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile all-intra encoded bitstream made up of 30 frames (128x72 resolution)</t>
-  </si>
-  <si>
-    <t>Convert an image to JPEG and extract the EXIF data as a blob file for further use</t>
-  </si>
-  <si>
-    <t>B014</t>
-  </si>
-  <si>
-    <t>A grid of 4 Images downsampled to 512x288 resolution and positioned to a 2x2 grid, then encoded as a single HD HEVC Main Profile bitstream.</t>
-  </si>
-  <si>
-    <t>B015</t>
-  </si>
-  <si>
-    <t>Image downsampled to 512x288 and then encoded using HEVC Main Profile</t>
-  </si>
-  <si>
-    <t>B016</t>
-  </si>
-  <si>
-    <t>Image downsampled to 512x288  and then encoded using HEVC Main Profile</t>
-  </si>
-  <si>
-    <t>B017</t>
-  </si>
-  <si>
-    <t>B018</t>
-  </si>
-  <si>
-    <t>1 HEVC Main Profile intra frame followed by 8 inter frames (1920x1080 resolution)</t>
-  </si>
-  <si>
-    <t>C034.exf</t>
-  </si>
-  <si>
-    <t>EXIF blob data for C034</t>
-  </si>
-  <si>
-    <t>C034.xmp</t>
-  </si>
-  <si>
-    <t>XMP blob data for C034</t>
+    <t xml:space="preserve">File ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input bitstreams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A file with an image item and an image sequence, using file offset, first image item a s primary image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B001, B002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heic, hevc, mif1, msf1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file with 1 image item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heic, mif1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file with 2 image items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B001, B003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file with 10 image items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thumbnail image as primary : one image and a thumbnail image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B001, B005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auxiliary image as a primary item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B001, B006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains a derived image of type "grid" from first 4 images and it is set as primary image item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains a derived image which is a rotated image of B003 input image and it is set as primary image item.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of the images is set as hidden image.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make these two items "altr" grouped.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make these items hidden and then "altr" grouped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file with 10 images, 10 thumbnails and 1 additional image item. Additional image item is pre-derived from two thumbnail images.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B004, B007, B001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clap box to crop (0,0,300,300) on 2 images  in C003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">irot box to rotate 90 degrees applied to one image  in C003 and then crop the image. Then, make that image a primary item. Add another irot box of 180 degree rotation and apply to B003 as another image item.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (160,240). Canvas fill is 0 (transparent)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a derived image item where the 1st image item is overlaid on a canvas of black. Total output w,h = 1440, 960. image on top of the first one with an offset of (80,120).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (640,360). Canvas fill is 65535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B008,B009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (640,360). Canvas fill is 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (-320,-180). Canvas fill is 65535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a derived image item where the 1st image item is overlaid on the second image. Total output w,h = 1440, 960.Second image on top of the first one with an offset of (-640,-360). Canvas fill is 65535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a derived image item where the  image item is overlaid on a canvas of dimensions w,h = 640, 360.Second image on top of the first one with an offset of (-640,-360). Canvas fill is 65535.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains a derived image of type "grid" from first 4 images and it is set as primary image item. Output width and height = (1449, 960)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">containes a grid of 4 derived images which are cropped to (640,360)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains a grid of 1x1 dimension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains a grid of 3x2 dimension. Uses the first 6 frames.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a file with an image sequence only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hevc, msf1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a file with image sequence track with inter prediction but no intra-pred in inter-predicted frames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a file with image sequence track with inter prediction with intra-pred in inter-predicted frames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A file with an edit list of playing the first 5 samples twice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A file with an edit list of a pause at the beginning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a file with image sequence track and a video track</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a file with a pict track and a thumbnail track also alternate groups indicated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B002, B012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a file with a pict track and a thumbnail track with no alternate groups indicated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A file with EXIF metadata present in it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mif1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A file with an all-intra encoded video track and an edit list with repeat flag, repeating an integer number of times.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A file with an all-intra encoded video track and an edit list with repeat flag, repeating a non-integer number of times.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A file with an all-intra encoded video track and an edit list with a repeat flag, repeating for infinite number of times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add another image item to C014 configuration with crop and rotate operation on top of already present crop-and-rotated image item and make that item a primary item.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-derived coded image. First 2x2 grid image as pre-derived coded image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B014, B015, B016, B017, B018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A file with a non-display sample (the first Intra frame) and 8 more inter-frames in it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitstream ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same input content as bitstream:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 HEVC Main Profile Intra encoded Frame (1280x720 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEVC Main Profile all-intra encoded bitstream made up of 8 frames (1280x720 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEVC Main Profile all-intra encoded bitstream made up of 10 frames (1280x720 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thumbail image - HEVC Main Profile Intra encoded Frame (128x72 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha mask of the image - HEVC Main Profile Intra encoded Frame (1280x720 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 HEVC Main Profile all-intra encoded bitstream made up of 10 frames (128x72 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 HEVC Main Profile all-Intra encoded Frame (640x360 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 HEVC Main Profile Intra encoded Frame (640x360 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEVC Main Profile inter-prediction used bitstream (1280x720 resolution) made up of 16 frames, but no intra-prediction in the inter-predicted frames.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEVC Main Profile inter-prediction used bitstream (1280x720 resolution) made up of 16 frames, with intra-prediction used in the inter-predicted frames.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEVC Main Profile all-intra encoded bitstream made up of 8 frames (128x72 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convert an image to JPEG and extract the EXIF data as a blob file for further use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A grid of 4 Images downsampled to 512x288 resolution and positioned to a 2x2 grid, then encoded as a single HD HEVC Main Profile bitstream.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image downsampled to 512x288 and then encoded using HEVC Main Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image downsampled to 512x288  and then encoded using HEVC Main Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 HEVC Main Profile intra frame followed by 8 inter frames (1920x1080 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C034.exf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXIF blob data for C034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C034.xmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XMP blob data for C034</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -635,20 +635,20 @@
   </sheetPr>
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="90.9433198380567"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.6315789473684"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4008097165992"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="91.6923076923077"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.0607287449393"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>67</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>108</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>17</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>71</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>74</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
Add multilayer conformance files.
</commit_message>
<xml_diff>
--- a/conformance_file_descriptions.xlsx
+++ b/conformance_file_descriptions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="159">
   <si>
     <t xml:space="preserve">File ID</t>
   </si>
@@ -334,6 +334,48 @@
     <t xml:space="preserve">B019</t>
   </si>
   <si>
+    <t xml:space="preserve">multilayer001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A base quality and an enhanced quality presentations of same image.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heic, heis, mif1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multilayer002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two image grid derived items, 2x2 each. Image items in the second grid have enhanced SNR.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multilayer003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A multi-view file with 'ster' grouping.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multilayer004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A base quality and an enhanced quality presenations of same image. The baselayer is an AVC-coded item.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B023, B024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heic, heis, mif1, avci</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bitstream ID</t>
   </si>
   <si>
@@ -431,6 +473,30 @@
   </si>
   <si>
     <t xml:space="preserve">XMP blob data for C034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 HEVC Scalable Main profile encoded frame, 2 layers, SNR scalability (1024x512 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 HEVC Scalable Main profile encoded frames, 2 layers, SNR scalability (512x256 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 HEVC Main profile intra encoded frames (1024x512 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 HEVC Scalable Main profile encoded enhancement layer for external baselayer, SNR scalability (1024x512 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 AVC encoded frame (1024x512 resolution)</t>
   </si>
 </sst>
 </file>
@@ -479,7 +545,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +556,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4F81BD"/>
         <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33FF99"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -530,7 +602,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -553,6 +625,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -608,7 +688,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF33FF99"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -633,18 +713,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="91.6923076923077"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.0607287449393"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5627530364372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1222,30 +1302,74 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0"/>
-    </row>
-    <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,7 +1377,7 @@
         <v>10</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,15 +1385,15 @@
         <v>67</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,15 +1401,15 @@
         <v>17</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>10</v>
@@ -1293,10 +1417,10 @@
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>10</v>
@@ -1307,7 +1431,7 @@
         <v>64</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>17</v>
@@ -1315,10 +1439,10 @@
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>10</v>
@@ -1326,13 +1450,13 @@
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1340,7 +1464,7 @@
         <v>71</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>67</v>
@@ -1351,7 +1475,7 @@
         <v>74</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>67</v>
@@ -1359,10 +1483,10 @@
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>67</v>
@@ -1373,7 +1497,7 @@
         <v>88</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>10</v>
@@ -1381,42 +1505,42 @@
     </row>
     <row r="61" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1424,25 +1548,77 @@
         <v>103</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update description sheet formatting.
</commit_message>
<xml_diff>
--- a/conformance_file_descriptions.xlsx
+++ b/conformance_file_descriptions.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">C002</t>
   </si>
   <si>
-    <t xml:space="preserve">file with 1 image item</t>
+    <t xml:space="preserve">File with 1 image item</t>
   </si>
   <si>
     <t xml:space="preserve">B001</t>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">C003</t>
   </si>
   <si>
-    <t xml:space="preserve">file with 2 image items</t>
+    <t xml:space="preserve">File with 2 image items</t>
   </si>
   <si>
     <t xml:space="preserve">B001, B003</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">C004</t>
   </si>
   <si>
-    <t xml:space="preserve">file with 10 image items</t>
+    <t xml:space="preserve">File with 10 image items</t>
   </si>
   <si>
     <t xml:space="preserve">B004</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">C005</t>
   </si>
   <si>
-    <t xml:space="preserve">thumbnail image as primary : one image and a thumbnail image</t>
+    <t xml:space="preserve">Thumbnail image as primary : one image and a thumbnail image</t>
   </si>
   <si>
     <t xml:space="preserve">B001, B005</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">C006</t>
   </si>
   <si>
-    <t xml:space="preserve">auxiliary image as a primary item</t>
+    <t xml:space="preserve">Auxiliary image as a primary item</t>
   </si>
   <si>
     <t xml:space="preserve">B001, B006</t>
@@ -97,13 +97,13 @@
     <t xml:space="preserve">C007</t>
   </si>
   <si>
-    <t xml:space="preserve">contains a derived image of type "grid" from first 4 images and it is set as primary image item</t>
+    <t xml:space="preserve">Contains a derived image of type "grid" from first 4 images and it is set as primary image item</t>
   </si>
   <si>
     <t xml:space="preserve">C008</t>
   </si>
   <si>
-    <t xml:space="preserve">contains a derived image which is a rotated image of B003 input image and it is set as primary image item.</t>
+    <t xml:space="preserve">Contains a derived image which is a rotated image of B003 input image and it is set as primary image item.</t>
   </si>
   <si>
     <t xml:space="preserve">C009</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">C012</t>
   </si>
   <si>
-    <t xml:space="preserve">file with 10 images, 10 thumbnails and 1 additional image item. Additional image item is pre-derived from two thumbnail images.</t>
+    <t xml:space="preserve">File with 10 images, 10 thumbnails and 1 additional image item. Additional image item is pre-derived from two thumbnail images.</t>
   </si>
   <si>
     <t xml:space="preserve">B004, B007, B001</t>
@@ -136,13 +136,13 @@
     <t xml:space="preserve">C013</t>
   </si>
   <si>
-    <t xml:space="preserve">clap box to crop (0,0,300,300) on 2 images  in C003</t>
+    <t xml:space="preserve">"clap" box to crop (0,0,300,300) on 2 images  in C003</t>
   </si>
   <si>
     <t xml:space="preserve">C014</t>
   </si>
   <si>
-    <t xml:space="preserve">irot box to rotate 90 degrees applied to one image  in C003 and then crop the image. Then, make that image a primary item. Add another irot box of 180 degree rotation and apply to B003 as another image item.</t>
+    <t xml:space="preserve">"irot" box to rotate 90 degrees applied to one image  in C003 and then crop the image. Then, make that image a primary item. Add another irot box of 180 degree rotation and apply to B003 as another image item.</t>
   </si>
   <si>
     <t xml:space="preserve">C015</t>
@@ -193,25 +193,25 @@
     <t xml:space="preserve">C022</t>
   </si>
   <si>
-    <t xml:space="preserve">contains a derived image of type "grid" from first 4 images and it is set as primary image item. Output width and height = (1449, 960)</t>
+    <t xml:space="preserve">Contains a derived image of type "grid" from first 4 images and it is set as primary image item. Output width and height = (1449, 960)</t>
   </si>
   <si>
     <t xml:space="preserve">C023</t>
   </si>
   <si>
-    <t xml:space="preserve">containes a grid of 4 derived images which are cropped to (640,360)</t>
+    <t xml:space="preserve">Contains a grid of 4 derived images which are cropped to (640,360)</t>
   </si>
   <si>
     <t xml:space="preserve">C024</t>
   </si>
   <si>
-    <t xml:space="preserve">contains a grid of 1x1 dimension</t>
+    <t xml:space="preserve">Contains a grid of 1x1 dimension</t>
   </si>
   <si>
     <t xml:space="preserve">C025</t>
   </si>
   <si>
-    <t xml:space="preserve">contains a grid of 3x2 dimension. Uses the first 6 frames.</t>
+    <t xml:space="preserve">Contains a grid of 3x2 dimension. Uses the first 6 frames.</t>
   </si>
   <si>
     <t xml:space="preserve">B007</t>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">C026</t>
   </si>
   <si>
-    <t xml:space="preserve">a file with an image sequence only</t>
+    <t xml:space="preserve">A file with an image sequence only</t>
   </si>
   <si>
     <t xml:space="preserve">B002</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">C027</t>
   </si>
   <si>
-    <t xml:space="preserve">a file with image sequence track with inter prediction but no intra-pred in inter-predicted frames</t>
+    <t xml:space="preserve">A file with image sequence track with inter prediction but no intra-pred in inter-predicted frames</t>
   </si>
   <si>
     <t xml:space="preserve">B010</t>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">C028</t>
   </si>
   <si>
-    <t xml:space="preserve">a file with image sequence track with inter prediction with intra-pred in inter-predicted frames</t>
+    <t xml:space="preserve">A file with image sequence track with inter prediction with intra-pred in inter-predicted frames</t>
   </si>
   <si>
     <t xml:space="preserve">B011</t>
@@ -262,13 +262,13 @@
     <t xml:space="preserve">C031</t>
   </si>
   <si>
-    <t xml:space="preserve">a file with image sequence track and a video track</t>
+    <t xml:space="preserve">A file with image sequence track and a video track</t>
   </si>
   <si>
     <t xml:space="preserve">C032</t>
   </si>
   <si>
-    <t xml:space="preserve">a file with a pict track and a thumbnail track also alternate groups indicated</t>
+    <t xml:space="preserve">A file with a pict track and a thumbnail track also alternate groups indicated</t>
   </si>
   <si>
     <t xml:space="preserve">B002, B012</t>
@@ -277,7 +277,7 @@
     <t xml:space="preserve">C033</t>
   </si>
   <si>
-    <t xml:space="preserve">a file with a pict track and a thumbnail track with no alternate groups indicated</t>
+    <t xml:space="preserve">A file with a pict track and a thumbnail track with no alternate groups indicated</t>
   </si>
   <si>
     <t xml:space="preserve">C034</t>
@@ -545,7 +545,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,12 +556,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4F81BD"/>
         <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF33FF99"/>
-        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -602,7 +596,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -625,14 +619,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -688,7 +674,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33FF99"/>
+      <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -713,22 +699,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5627530364372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="92.4453441295547"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5951417004049"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3238866396761"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="103.963562753036"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.004048582996"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1821862348178"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.25506072874494"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -742,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -756,7 +742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
@@ -770,7 +756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
@@ -784,7 +770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
@@ -798,7 +784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
@@ -812,7 +798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>21</v>
       </c>
@@ -826,7 +812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>24</v>
       </c>
@@ -840,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>26</v>
       </c>
@@ -854,7 +840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>28</v>
       </c>
@@ -868,7 +854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>30</v>
       </c>
@@ -882,7 +868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>32</v>
       </c>
@@ -896,7 +882,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>34</v>
       </c>
@@ -910,7 +896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>37</v>
       </c>
@@ -924,7 +910,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>39</v>
       </c>
@@ -938,7 +924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>41</v>
       </c>
@@ -952,7 +938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>43</v>
       </c>
@@ -966,7 +952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>45</v>
       </c>
@@ -980,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>48</v>
       </c>
@@ -994,7 +980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>50</v>
       </c>
@@ -1008,7 +994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>52</v>
       </c>
@@ -1022,7 +1008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>54</v>
       </c>
@@ -1036,7 +1022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>56</v>
       </c>
@@ -1050,7 +1036,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>58</v>
       </c>
@@ -1064,7 +1050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>60</v>
       </c>
@@ -1078,7 +1064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>62</v>
       </c>
@@ -1092,7 +1078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>65</v>
       </c>
@@ -1106,7 +1092,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>69</v>
       </c>
@@ -1120,7 +1106,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>72</v>
       </c>
@@ -1134,7 +1120,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>75</v>
       </c>
@@ -1148,7 +1134,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>77</v>
       </c>
@@ -1162,7 +1148,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>79</v>
       </c>
@@ -1176,7 +1162,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>81</v>
       </c>
@@ -1190,7 +1176,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>84</v>
       </c>
@@ -1204,7 +1190,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>86</v>
       </c>
@@ -1218,7 +1204,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>90</v>
       </c>
@@ -1232,7 +1218,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>92</v>
       </c>
@@ -1246,7 +1232,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>94</v>
       </c>
@@ -1260,7 +1246,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>96</v>
       </c>
@@ -1274,11 +1260,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C40" s="0" t="s">
@@ -1288,80 +1274,80 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="0" t="s">
         <v>103</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="0" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="0" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="s">
+      <c r="D44" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="0" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="0"/>
     </row>
-    <row r="47" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>118</v>
       </c>
@@ -1372,7 +1358,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>10</v>
       </c>
@@ -1380,7 +1366,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>67</v>
       </c>
@@ -1388,7 +1374,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>122</v>
       </c>
@@ -1396,7 +1382,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>17</v>
       </c>
@@ -1404,7 +1390,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>124</v>
       </c>
@@ -1415,7 +1401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>126</v>
       </c>
@@ -1426,7 +1412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>64</v>
       </c>
@@ -1437,7 +1423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>129</v>
       </c>
@@ -1448,7 +1434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>131</v>
       </c>
@@ -1459,7 +1445,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>71</v>
       </c>
@@ -1470,7 +1456,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>74</v>
       </c>
@@ -1481,7 +1467,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>135</v>
       </c>
@@ -1492,7 +1478,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>88</v>
       </c>
@@ -1503,7 +1489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>138</v>
       </c>
@@ -1511,7 +1497,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>140</v>
       </c>
@@ -1519,7 +1505,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>142</v>
       </c>
@@ -1527,7 +1513,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>144</v>
       </c>
@@ -1535,7 +1521,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>145</v>
       </c>
@@ -1543,7 +1529,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
         <v>103</v>
       </c>
@@ -1551,7 +1537,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>147</v>
       </c>
@@ -1559,66 +1545,63 @@
         <v>148</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="s">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C69" s="6"/>
-    </row>
-    <row r="70" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6" t="s">
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="0" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6" t="s">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C71" s="6"/>
-    </row>
-    <row r="72" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="6" t="s">
+    </row>
+    <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="0" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="6" t="s">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="0" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add new conformance files.
</commit_message>
<xml_diff>
--- a/conformance_file_descriptions.xlsx
+++ b/conformance_file_descriptions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="166">
   <si>
     <t xml:space="preserve">File ID</t>
   </si>
@@ -334,6 +334,12 @@
     <t xml:space="preserve">B019</t>
   </si>
   <si>
+    <t xml:space="preserve">C042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An image item vertically mirrored with an "imir" property.</t>
+  </si>
+  <si>
     <t xml:space="preserve">multilayer001</t>
   </si>
   <si>
@@ -376,6 +382,15 @@
     <t xml:space="preserve">heic, heis, mif1, avci</t>
   </si>
   <si>
+    <t xml:space="preserve">multilayer005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A multi-layer multiview file with 'ster' grouping.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B025</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bitstream ID</t>
   </si>
   <si>
@@ -497,6 +512,12 @@
   </si>
   <si>
     <t xml:space="preserve">1 AVC encoded frame (1024x512 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 HEVC encoded multi-layer frame. Layer 0 is the left view, layer 1 is the right view.  (512x256 resolution)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B22</t>
   </si>
 </sst>
 </file>
@@ -699,19 +720,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3238866396761"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="103.963562753036"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.004048582996"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.25506072874494"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="104.87044534413"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1288,147 +1309,153 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="4" t="s">
         <v>105</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="D43" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="D44" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="D45" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0"/>
-    </row>
-    <row r="47" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
+      <c r="C46" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="D46" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>121</v>
+      <c r="C49" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>122</v>
+        <v>10</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>126</v>
+        <v>17</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>10</v>
@@ -1436,170 +1463,203 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="B59" s="4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>142</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
-        <v>103</v>
+      <c r="A66" s="0" t="s">
+        <v>149</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>150</v>
+      <c r="A68" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C74" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="C73" s="0" t="s">
-        <v>153</v>
+    </row>
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update files C006.heic and C052.heic.
Changelog:
-Update files C006.heic and C052.heic to contain intended coded auxiliary image item data.
-Update C006.heic to signal the master image as the primary item.
-Update description sheet.
</commit_message>
<xml_diff>
--- a/conformance_file_descriptions.xlsx
+++ b/conformance_file_descriptions.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">C006</t>
   </si>
   <si>
-    <t xml:space="preserve">An image item with an associated alpha mask auxiliary image. Auxiliary image as the primary item.</t>
+    <t xml:space="preserve">An image item with an associated alpha mask auxiliary image.</t>
   </si>
   <si>
     <t xml:space="preserve">B001, B006</t>
@@ -851,7 +851,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -877,10 +877,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -966,7 +962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1783,13 +1779,13 @@
       <c r="F55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="4" t="s">
         <v>152</v>
       </c>
       <c r="D56" s="4" t="s">
@@ -1799,13 +1795,13 @@
       <c r="F56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D57" s="4" t="s">
@@ -1815,13 +1811,13 @@
       <c r="F57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="4" t="s">
         <v>159</v>
       </c>
       <c r="D58" s="4" t="s">
@@ -1831,13 +1827,13 @@
       <c r="F58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="4" t="s">
         <v>159</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -1847,13 +1843,13 @@
       <c r="F59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="4" t="s">
         <v>165</v>
       </c>
       <c r="D60" s="4" t="s">
@@ -1863,13 +1859,13 @@
       <c r="F60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="4" t="s">
         <v>169</v>
       </c>
       <c r="D61" s="4" t="s">
@@ -2221,47 +2217,47 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B98" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C98" s="7"/>
+      <c r="C98" s="4"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="7" t="s">
+      <c r="A99" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B99" s="8" t="s">
+      <c r="B99" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="C99" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D99" s="9"/>
+      <c r="D99" s="8"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="7" t="s">
+      <c r="A100" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D100" s="9"/>
+      <c r="D100" s="8"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B101" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="C101" s="7"/>
-      <c r="D101" s="9"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="8"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">

</xml_diff>